<commit_message>
+ update(sql): adding sql support for user login in
</commit_message>
<xml_diff>
--- a/SQL/SQL_Data.xlsx
+++ b/SQL/SQL_Data.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="20490" windowHeight="8340" firstSheet="1" activeTab="6"/>
+    <workbookView windowWidth="20490" windowHeight="7710" firstSheet="1" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="Department" sheetId="1" r:id="rId1"/>
@@ -15,13 +15,14 @@
     <sheet name="ExClass" sheetId="6" r:id="rId6"/>
     <sheet name="Learn" sheetId="7" r:id="rId7"/>
     <sheet name="Teaching" sheetId="8" r:id="rId8"/>
+    <sheet name="Admin" sheetId="9" r:id="rId9"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="305" uniqueCount="112">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="329" uniqueCount="133">
   <si>
     <t>DeptNo</t>
   </si>
@@ -92,21 +93,54 @@
     <t>TechName</t>
   </si>
   <si>
+    <t>Pwd</t>
+  </si>
+  <si>
+    <t>20200010001</t>
+  </si>
+  <si>
     <t>Jacky</t>
   </si>
   <si>
+    <t>123456</t>
+  </si>
+  <si>
+    <t>20200010002</t>
+  </si>
+  <si>
     <t>Gary</t>
   </si>
   <si>
+    <t>123457</t>
+  </si>
+  <si>
+    <t>20200010003</t>
+  </si>
+  <si>
     <t>Paul</t>
   </si>
   <si>
+    <t>123458</t>
+  </si>
+  <si>
+    <t>20200010004</t>
+  </si>
+  <si>
     <t>Toby</t>
   </si>
   <si>
+    <t>123459</t>
+  </si>
+  <si>
+    <t>20200010005</t>
+  </si>
+  <si>
     <t>Tony</t>
   </si>
   <si>
+    <t>123460</t>
+  </si>
+  <si>
     <t>StuNo</t>
   </si>
   <si>
@@ -131,27 +165,51 @@
     <t>gary</t>
   </si>
   <si>
+    <t>123461</t>
+  </si>
+  <si>
     <t>paul</t>
   </si>
   <si>
+    <t>123462</t>
+  </si>
+  <si>
     <t>khan</t>
   </si>
   <si>
+    <t>123463</t>
+  </si>
+  <si>
     <t>tiantian</t>
   </si>
   <si>
+    <t>123464</t>
+  </si>
+  <si>
     <t>god</t>
   </si>
   <si>
+    <t>123465</t>
+  </si>
+  <si>
     <t>black</t>
   </si>
   <si>
+    <t>123466</t>
+  </si>
+  <si>
     <t>blue</t>
   </si>
   <si>
+    <t>123467</t>
+  </si>
+  <si>
     <t>pink</t>
   </si>
   <si>
+    <t>123468</t>
+  </si>
+  <si>
     <t>CourseNo</t>
   </si>
   <si>
@@ -357,6 +415,12 @@
   </si>
   <si>
     <t>Grade</t>
+  </si>
+  <si>
+    <t>ID</t>
+  </si>
+  <si>
+    <t>Password</t>
   </si>
 </sst>
 </file>
@@ -364,10 +428,10 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="4">
-    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
     <numFmt numFmtId="42" formatCode="_ &quot;￥&quot;* #,##0_ ;_ &quot;￥&quot;* \-#,##0_ ;_ &quot;￥&quot;* &quot;-&quot;_ ;_ @_ "/>
     <numFmt numFmtId="41" formatCode="_ * #,##0_ ;_ * \-#,##0_ ;_ * &quot;-&quot;_ ;_ @_ "/>
-    <numFmt numFmtId="43" formatCode="_ * #,##0.00_ ;_ * \-#,##0.00_ ;_ * &quot;-&quot;??_ ;_ @_ "/>
+    <numFmt numFmtId="44" formatCode="_ &quot;￥&quot;* #,##0.00_ ;_ &quot;￥&quot;* \-#,##0.00_ ;_ &quot;￥&quot;* &quot;-&quot;??_ ;_ @_ "/>
   </numFmts>
   <fonts count="20">
     <font>
@@ -386,6 +450,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color theme="1"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
       <color theme="0"/>
       <name val="宋体"/>
       <charset val="0"/>
@@ -393,23 +464,15 @@
     </font>
     <font>
       <b/>
-      <sz val="13"/>
+      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
       <scheme val="minor"/>
     </font>
     <font>
-      <u/>
       <sz val="11"/>
-      <color rgb="FF0000FF"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
+      <color rgb="FFFF0000"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -417,14 +480,6 @@
     <font>
       <b/>
       <sz val="18"/>
-      <color theme="3"/>
-      <name val="宋体"/>
-      <charset val="134"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -462,15 +517,8 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color rgb="FF006100"/>
-      <name val="宋体"/>
-      <charset val="0"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <b/>
-      <sz val="15"/>
+      <sz val="13"/>
       <color theme="3"/>
       <name val="宋体"/>
       <charset val="134"/>
@@ -480,6 +528,14 @@
       <b/>
       <sz val="11"/>
       <color rgb="FFFA7D00"/>
+      <name val="宋体"/>
+      <charset val="0"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color rgb="FF0000FF"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -500,8 +556,16 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="宋体"/>
+      <charset val="134"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF006100"/>
       <name val="宋体"/>
       <charset val="0"/>
       <scheme val="minor"/>
@@ -531,13 +595,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9"/>
+        <fgColor theme="4" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.399975585192419"/>
+        <fgColor theme="8" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.599993896298105"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -561,25 +643,31 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="7" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.799981688894314"/>
+        <fgColor rgb="FFF2F2F2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -597,13 +685,43 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
+        <fgColor theme="9" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="6" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
         <fgColor theme="4"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.799981688894314"/>
+        <fgColor theme="7" tint="0.399975585192419"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -615,7 +733,25 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.399975585192419"/>
+        <fgColor theme="5" tint="0.799981688894314"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFEB9C"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="7"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -627,91 +763,19 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFFEB9C"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.799981688894314"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.399975585192419"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="4" tint="0.599993896298105"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6" tint="0.799981688894314"/>
+        <fgColor theme="8" tint="0.399975585192419"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFFFCC99"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="6"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.599993896298105"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -734,15 +798,6 @@
       <diagonal/>
     </border>
     <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
       <left style="thin">
         <color rgb="FFB2B2B2"/>
       </left>
@@ -754,6 +809,15 @@
       </top>
       <bottom style="thin">
         <color rgb="FFB2B2B2"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4" tint="0.499984740745262"/>
       </bottom>
       <diagonal/>
     </border>
@@ -788,6 +852,15 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
         <color rgb="FF7F7F7F"/>
       </left>
@@ -813,159 +886,150 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top/>
-      <bottom style="medium">
-        <color theme="4" tint="0.499984740745262"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="3" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="32" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="12" fillId="13" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="15" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="13" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="30" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="10" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="12" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="0" borderId="7" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="11" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="10" borderId="4" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="42" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="43" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="18" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="6" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="41" fontId="0" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -1342,7 +1406,7 @@
       <selection activeCell="C23" sqref="C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelRow="6" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="6" outlineLevelCol="1"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
@@ -1419,7 +1483,7 @@
       <selection activeCell="C2" sqref="C2:C6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="16384" width="9" style="1"/>
   </cols>
@@ -1551,18 +1615,19 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C6"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C8" sqref="C8"/>
+      <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9" defaultRowHeight="16.5" outlineLevelRow="5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelRow="5" outlineLevelCol="3"/>
   <cols>
-    <col min="1" max="16384" width="9" style="1"/>
+    <col min="1" max="1" width="12.625" style="1" customWidth="1"/>
+    <col min="2" max="16384" width="9" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="3" t="s">
         <v>21</v>
       </c>
@@ -1572,60 +1637,78 @@
       <c r="C1" s="3" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="3" t="s">
-        <v>2</v>
+        <v>24</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C2" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="3" t="s">
-        <v>4</v>
+        <v>27</v>
       </c>
       <c r="B3" s="3" t="s">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="3" t="s">
-        <v>6</v>
+        <v>30</v>
       </c>
       <c r="B4" s="3" t="s">
-        <v>25</v>
+        <v>31</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="3" t="s">
-        <v>8</v>
+        <v>33</v>
       </c>
       <c r="B5" s="3" t="s">
-        <v>26</v>
+        <v>34</v>
       </c>
       <c r="C5" s="3" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="3" t="s">
-        <v>10</v>
+        <v>36</v>
       </c>
       <c r="B6" s="3" t="s">
-        <v>27</v>
+        <v>37</v>
       </c>
       <c r="C6" s="3" t="s">
         <v>10</v>
+      </c>
+      <c r="D6" s="1" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>
@@ -1638,170 +1721,212 @@
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C15" sqref="C15"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H5" sqref="H5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="16.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="15" outlineLevelCol="3"/>
   <cols>
     <col min="1" max="1" width="12.1333333333333" style="2"/>
     <col min="2" max="16384" width="9.06666666666667" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:4">
       <c r="A1" s="2" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>29</v>
+        <v>40</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="2" spans="1:3">
+      <c r="D1" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4">
       <c r="A2" s="2">
         <v>20200740001</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>30</v>
+        <v>41</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="3" spans="1:3">
+      <c r="D2" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
       <c r="A3" s="2">
         <v>20200740002</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="4" spans="1:3">
+      <c r="D3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
       <c r="A4" s="2">
         <v>20200740003</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="5" spans="1:3">
+      <c r="D4" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
       <c r="A5" s="2">
         <v>20200740004</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:3">
+      <c r="D5" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
       <c r="A6" s="2">
         <v>20200740005</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="7" spans="1:3">
+      <c r="D6" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
       <c r="A7" s="2">
         <v>20200740006</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>35</v>
+        <v>46</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="8" spans="1:3">
+      <c r="D7" s="1" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
       <c r="A8" s="2">
         <v>20200740007</v>
       </c>
       <c r="B8" s="1" t="s">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="9" spans="1:3">
+      <c r="D8" s="1" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
       <c r="A9" s="2">
         <v>20200740008</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>37</v>
+        <v>50</v>
       </c>
       <c r="C9" s="1" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="10" spans="1:3">
+      <c r="D9" s="1" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
       <c r="A10" s="2">
         <v>20200740009</v>
       </c>
       <c r="B10" s="1" t="s">
-        <v>38</v>
+        <v>52</v>
       </c>
       <c r="C10" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="11" spans="1:3">
+      <c r="D10" s="1" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
       <c r="A11" s="2">
         <v>20200740010</v>
       </c>
       <c r="B11" s="1" t="s">
-        <v>39</v>
+        <v>54</v>
       </c>
       <c r="C11" s="1" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="12" spans="1:3">
+      <c r="D11" s="1" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
       <c r="A12" s="2">
         <v>20200740011</v>
       </c>
       <c r="B12" s="1" t="s">
-        <v>40</v>
+        <v>56</v>
       </c>
       <c r="C12" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="13" spans="1:3">
+      <c r="D12" s="1" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
       <c r="A13" s="2">
         <v>20200740012</v>
       </c>
       <c r="B13" s="1" t="s">
-        <v>41</v>
+        <v>58</v>
       </c>
       <c r="C13" s="1" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="14" spans="1:3">
+      <c r="D13" s="1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
       <c r="A14" s="2">
         <v>20200740013</v>
       </c>
       <c r="B14" s="1" t="s">
-        <v>42</v>
+        <v>60</v>
       </c>
       <c r="C14" s="1" t="s">
         <v>2</v>
+      </c>
+      <c r="D14" s="1" t="s">
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1819,19 +1944,19 @@
       <selection activeCell="C8" sqref="C8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="16.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="15" outlineLevelCol="1"/>
   <sheetData>
     <row r="1" spans="1:2">
       <c r="A1" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="B1" t="s">
-        <v>44</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="4" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B2" t="s">
         <v>3</v>
@@ -1839,58 +1964,58 @@
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="4" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="B3" t="s">
-        <v>47</v>
+        <v>66</v>
       </c>
     </row>
     <row r="4" spans="1:2">
       <c r="A4" s="4" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="B4" t="s">
-        <v>49</v>
+        <v>68</v>
       </c>
     </row>
     <row r="5" spans="1:2">
       <c r="A5" s="4" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="B5" t="s">
-        <v>51</v>
+        <v>70</v>
       </c>
     </row>
     <row r="6" spans="1:2">
       <c r="A6" s="4" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>72</v>
       </c>
     </row>
     <row r="7" spans="1:2">
       <c r="A7" s="4" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="B7" t="s">
-        <v>55</v>
+        <v>74</v>
       </c>
     </row>
     <row r="8" spans="1:2">
       <c r="A8" s="4" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B8" t="s">
-        <v>57</v>
+        <v>76</v>
       </c>
     </row>
     <row r="9" spans="1:2">
       <c r="A9" s="4" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="B9" t="s">
-        <v>59</v>
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1904,780 +2029,780 @@
   <sheetPr/>
   <dimension ref="A1:D55"/>
   <sheetViews>
-    <sheetView zoomScale="85" zoomScaleNormal="85" topLeftCell="A34" workbookViewId="0">
+    <sheetView zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
       <selection activeCell="B2" sqref="B2:B19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="16.5" outlineLevelCol="3"/>
+  <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="15" outlineLevelCol="3"/>
   <sheetData>
     <row r="1" spans="1:4">
       <c r="A1" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="B1" t="s">
-        <v>43</v>
+        <v>62</v>
       </c>
       <c r="C1" t="s">
-        <v>61</v>
+        <v>80</v>
       </c>
       <c r="D1" t="s">
-        <v>62</v>
+        <v>81</v>
       </c>
     </row>
     <row r="2" spans="1:4">
       <c r="A2" s="4" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C2">
         <v>2020</v>
       </c>
       <c r="D2" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="3" spans="1:4">
       <c r="A3" s="4" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C3">
         <v>2020</v>
       </c>
       <c r="D3" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:4">
       <c r="A4" s="4" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="C4">
         <v>2020</v>
       </c>
       <c r="D4" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="5" spans="1:4">
       <c r="A5" s="4" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C5">
         <v>2020</v>
       </c>
       <c r="D5" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="6" spans="1:4">
       <c r="A6" s="4" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="C6">
         <v>2020</v>
       </c>
       <c r="D6" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="7" spans="1:4">
       <c r="A7" s="4" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C7">
         <v>2020</v>
       </c>
       <c r="D7" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="8" spans="1:4">
       <c r="A8" s="4" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C8">
         <v>2020</v>
       </c>
       <c r="D8" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="9" spans="1:4">
       <c r="A9" s="4" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C9">
         <v>2020</v>
       </c>
       <c r="D9" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="10" spans="1:4">
       <c r="A10" s="4" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="C10">
         <v>2020</v>
       </c>
       <c r="D10" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="11" spans="1:4">
       <c r="A11" s="4" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C11">
         <v>2020</v>
       </c>
       <c r="D11" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="12" spans="1:4">
       <c r="A12" s="4" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="C12">
         <v>2020</v>
       </c>
       <c r="D12" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="13" spans="1:4">
       <c r="A13" s="4" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C13">
         <v>2020</v>
       </c>
       <c r="D13" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="14" spans="1:4">
       <c r="A14" s="4" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="C14">
         <v>2020</v>
       </c>
       <c r="D14" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="15" spans="1:4">
       <c r="A15" s="4" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="C15">
         <v>2020</v>
       </c>
       <c r="D15" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="16" spans="1:4">
       <c r="A16" s="4" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C16">
         <v>2020</v>
       </c>
       <c r="D16" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="17" spans="1:4">
       <c r="A17" s="4" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C17">
         <v>2020</v>
       </c>
       <c r="D17" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="18" spans="1:4">
       <c r="A18" s="4" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="C18">
         <v>2020</v>
       </c>
       <c r="D18" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="19" spans="1:4">
       <c r="A19" s="4" t="s">
-        <v>74</v>
+        <v>93</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C19">
         <v>2020</v>
       </c>
       <c r="D19" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="20" spans="1:4">
       <c r="A20" s="4" t="s">
-        <v>75</v>
+        <v>94</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="C20">
         <v>2020</v>
       </c>
       <c r="D20" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:4">
       <c r="A21" s="4" t="s">
-        <v>76</v>
+        <v>95</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C21">
         <v>2020</v>
       </c>
       <c r="D21" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="22" spans="1:4">
       <c r="A22" s="4" t="s">
-        <v>77</v>
+        <v>96</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C22">
         <v>2020</v>
       </c>
       <c r="D22" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:4">
       <c r="A23" s="4" t="s">
-        <v>78</v>
+        <v>97</v>
       </c>
       <c r="B23" s="4" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C23">
         <v>2020</v>
       </c>
       <c r="D23" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="24" spans="1:4">
       <c r="A24" s="4" t="s">
-        <v>79</v>
+        <v>98</v>
       </c>
       <c r="B24" s="4" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="C24">
         <v>2020</v>
       </c>
       <c r="D24" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="25" spans="1:4">
       <c r="A25" s="4" t="s">
-        <v>80</v>
+        <v>99</v>
       </c>
       <c r="B25" s="4" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C25">
         <v>2020</v>
       </c>
       <c r="D25" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="26" spans="1:4">
       <c r="A26" s="4" t="s">
-        <v>81</v>
+        <v>100</v>
       </c>
       <c r="B26" s="4" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="C26">
         <v>2020</v>
       </c>
       <c r="D26" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:4">
       <c r="A27" s="4" t="s">
-        <v>82</v>
+        <v>101</v>
       </c>
       <c r="B27" s="4" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C27">
         <v>2020</v>
       </c>
       <c r="D27" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="28" spans="1:4">
       <c r="A28" s="4" t="s">
-        <v>83</v>
+        <v>102</v>
       </c>
       <c r="B28" s="4" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="C28">
         <v>2020</v>
       </c>
       <c r="D28" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="29" spans="1:4">
       <c r="A29" s="4" t="s">
-        <v>84</v>
+        <v>103</v>
       </c>
       <c r="B29" s="4" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="C29">
         <v>2021</v>
       </c>
       <c r="D29" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="30" spans="1:4">
       <c r="A30" s="4" t="s">
-        <v>85</v>
+        <v>104</v>
       </c>
       <c r="B30" s="4" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C30">
         <v>2021</v>
       </c>
       <c r="D30" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="31" spans="1:4">
       <c r="A31" s="4" t="s">
-        <v>86</v>
+        <v>105</v>
       </c>
       <c r="B31" s="4" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="C31">
         <v>2021</v>
       </c>
       <c r="D31" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="32" spans="1:4">
       <c r="A32" s="4" t="s">
-        <v>87</v>
+        <v>106</v>
       </c>
       <c r="B32" s="4" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C32">
         <v>2021</v>
       </c>
       <c r="D32" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="33" spans="1:4">
       <c r="A33" s="4" t="s">
-        <v>88</v>
+        <v>107</v>
       </c>
       <c r="B33" s="4" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C33">
         <v>2021</v>
       </c>
       <c r="D33" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="34" spans="1:4">
       <c r="A34" s="4" t="s">
-        <v>89</v>
+        <v>108</v>
       </c>
       <c r="B34" s="4" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C34">
         <v>2021</v>
       </c>
       <c r="D34" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="35" spans="1:4">
       <c r="A35" s="4" t="s">
-        <v>90</v>
+        <v>109</v>
       </c>
       <c r="B35" s="4" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="C35">
         <v>2021</v>
       </c>
       <c r="D35" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="36" spans="1:4">
       <c r="A36" s="4" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="B36" s="4" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C36">
         <v>2021</v>
       </c>
       <c r="D36" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="37" spans="1:4">
       <c r="A37" s="4" t="s">
-        <v>92</v>
+        <v>111</v>
       </c>
       <c r="B37" s="4" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="C37">
         <v>2021</v>
       </c>
       <c r="D37" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="38" spans="1:4">
       <c r="A38" s="4" t="s">
-        <v>93</v>
+        <v>112</v>
       </c>
       <c r="B38" s="4" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C38">
         <v>2021</v>
       </c>
       <c r="D38" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="39" spans="1:4">
       <c r="A39" s="4" t="s">
-        <v>94</v>
+        <v>113</v>
       </c>
       <c r="B39" s="4" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="C39">
         <v>2021</v>
       </c>
       <c r="D39" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="40" spans="1:4">
       <c r="A40" s="4" t="s">
-        <v>95</v>
+        <v>114</v>
       </c>
       <c r="B40" s="4" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="C40">
         <v>2021</v>
       </c>
       <c r="D40" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="41" spans="1:4">
       <c r="A41" s="4" t="s">
-        <v>96</v>
+        <v>115</v>
       </c>
       <c r="B41" s="4" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C41">
         <v>2021</v>
       </c>
       <c r="D41" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="42" spans="1:4">
       <c r="A42" s="4" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="B42" s="4" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C42">
         <v>2021</v>
       </c>
       <c r="D42" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="43" spans="1:4">
       <c r="A43" s="4" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="B43" s="4" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="C43">
         <v>2021</v>
       </c>
       <c r="D43" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="44" spans="1:4">
       <c r="A44" s="4" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="B44" s="4" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C44">
         <v>2021</v>
       </c>
       <c r="D44" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="45" spans="1:4">
       <c r="A45" s="4" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="B45" s="4" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="C45">
         <v>2021</v>
       </c>
       <c r="D45" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="46" spans="1:4">
       <c r="A46" s="4" t="s">
-        <v>101</v>
+        <v>120</v>
       </c>
       <c r="B46" s="4" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C46">
         <v>2021</v>
       </c>
       <c r="D46" t="s">
-        <v>63</v>
+        <v>82</v>
       </c>
     </row>
     <row r="47" spans="1:4">
       <c r="A47" s="4" t="s">
-        <v>102</v>
+        <v>121</v>
       </c>
       <c r="B47" s="4" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C47">
         <v>2021</v>
       </c>
       <c r="D47" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="48" spans="1:4">
       <c r="A48" s="4" t="s">
-        <v>103</v>
+        <v>122</v>
       </c>
       <c r="B48" s="4" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C48">
         <v>2021</v>
       </c>
       <c r="D48" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="49" spans="1:4">
       <c r="A49" s="4" t="s">
-        <v>104</v>
+        <v>123</v>
       </c>
       <c r="B49" s="4" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="C49">
         <v>2021</v>
       </c>
       <c r="D49" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="50" spans="1:4">
       <c r="A50" s="4" t="s">
-        <v>105</v>
+        <v>124</v>
       </c>
       <c r="B50" s="4" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C50">
         <v>2021</v>
       </c>
       <c r="D50" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="51" spans="1:4">
       <c r="A51" s="4" t="s">
-        <v>106</v>
+        <v>125</v>
       </c>
       <c r="B51" s="4" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="C51">
         <v>2021</v>
       </c>
       <c r="D51" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="52" spans="1:4">
       <c r="A52" s="4" t="s">
-        <v>107</v>
+        <v>126</v>
       </c>
       <c r="B52" s="4" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C52">
         <v>2021</v>
       </c>
       <c r="D52" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="53" spans="1:4">
       <c r="A53" s="4" t="s">
-        <v>108</v>
+        <v>127</v>
       </c>
       <c r="B53" s="4" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C53">
         <v>2021</v>
       </c>
       <c r="D53" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="54" spans="1:4">
       <c r="A54" s="4" t="s">
-        <v>109</v>
+        <v>128</v>
       </c>
       <c r="B54" s="4" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C54">
         <v>2021</v>
       </c>
       <c r="D54" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
     <row r="55" spans="1:4">
       <c r="A55" s="4" t="s">
-        <v>110</v>
+        <v>129</v>
       </c>
       <c r="B55" s="4" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="C55">
         <v>2021</v>
       </c>
       <c r="D55" t="s">
-        <v>73</v>
+        <v>92</v>
       </c>
     </row>
   </sheetData>
@@ -2691,24 +2816,24 @@
   <sheetPr/>
   <dimension ref="A1:C22"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A23" sqref="A23:C23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="16.5" outlineLevelCol="2"/>
+  <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="15" outlineLevelCol="2"/>
   <cols>
     <col min="1" max="1" width="12.1333333333333"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3">
       <c r="A1" t="s">
-        <v>28</v>
+        <v>39</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>79</v>
       </c>
       <c r="C1" t="s">
-        <v>111</v>
+        <v>130</v>
       </c>
     </row>
     <row r="2" spans="1:3">
@@ -2716,7 +2841,7 @@
         <v>20200740001</v>
       </c>
       <c r="B2" s="4" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C2">
         <v>86.36</v>
@@ -2727,7 +2852,7 @@
         <v>20200740002</v>
       </c>
       <c r="B3" s="4" t="s">
-        <v>46</v>
+        <v>65</v>
       </c>
       <c r="C3">
         <v>74.47</v>
@@ -2738,7 +2863,7 @@
         <v>20200740003</v>
       </c>
       <c r="B4" s="4" t="s">
-        <v>48</v>
+        <v>67</v>
       </c>
       <c r="C4">
         <v>53.78</v>
@@ -2749,7 +2874,7 @@
         <v>20200740004</v>
       </c>
       <c r="B5" s="4" t="s">
-        <v>50</v>
+        <v>69</v>
       </c>
       <c r="C5">
         <v>83.48</v>
@@ -2760,7 +2885,7 @@
         <v>20200740005</v>
       </c>
       <c r="B6" s="4" t="s">
-        <v>52</v>
+        <v>71</v>
       </c>
       <c r="C6">
         <v>37.57</v>
@@ -2771,7 +2896,7 @@
         <v>20200740006</v>
       </c>
       <c r="B7" s="4" t="s">
-        <v>54</v>
+        <v>73</v>
       </c>
       <c r="C7">
         <v>89.25</v>
@@ -2782,7 +2907,7 @@
         <v>20200740007</v>
       </c>
       <c r="B8" s="4" t="s">
-        <v>56</v>
+        <v>75</v>
       </c>
       <c r="C8">
         <v>90.47</v>
@@ -2793,7 +2918,7 @@
         <v>20200740008</v>
       </c>
       <c r="B9" s="4" t="s">
-        <v>58</v>
+        <v>77</v>
       </c>
       <c r="C9">
         <v>99.99</v>
@@ -2804,7 +2929,7 @@
         <v>20200740009</v>
       </c>
       <c r="B10" s="4" t="s">
-        <v>64</v>
+        <v>83</v>
       </c>
       <c r="C10">
         <v>87.58</v>
@@ -2815,7 +2940,7 @@
         <v>20200740010</v>
       </c>
       <c r="B11" s="4" t="s">
-        <v>65</v>
+        <v>84</v>
       </c>
       <c r="C11">
         <v>78.78</v>
@@ -2826,7 +2951,7 @@
         <v>20200740011</v>
       </c>
       <c r="B12" s="4" t="s">
-        <v>66</v>
+        <v>85</v>
       </c>
       <c r="C12">
         <v>75.38</v>
@@ -2837,7 +2962,7 @@
         <v>20200740012</v>
       </c>
       <c r="B13" s="4" t="s">
-        <v>67</v>
+        <v>86</v>
       </c>
       <c r="C13">
         <v>38.8</v>
@@ -2848,7 +2973,7 @@
         <v>20200740013</v>
       </c>
       <c r="B14" s="4" t="s">
-        <v>68</v>
+        <v>87</v>
       </c>
       <c r="C14">
         <v>89.45</v>
@@ -2859,7 +2984,7 @@
         <v>20200740012</v>
       </c>
       <c r="B15" s="4" t="s">
-        <v>69</v>
+        <v>88</v>
       </c>
       <c r="C15">
         <v>80.95</v>
@@ -2870,7 +2995,7 @@
         <v>20200740001</v>
       </c>
       <c r="B16" s="4" t="s">
-        <v>70</v>
+        <v>89</v>
       </c>
       <c r="C16">
         <v>78.78</v>
@@ -2881,7 +3006,7 @@
         <v>20200740001</v>
       </c>
       <c r="B17" s="4" t="s">
-        <v>71</v>
+        <v>90</v>
       </c>
       <c r="C17">
         <v>75.38</v>
@@ -2892,7 +3017,7 @@
         <v>20200740001</v>
       </c>
       <c r="B18" s="4" t="s">
-        <v>72</v>
+        <v>91</v>
       </c>
       <c r="C18">
         <v>38.8</v>
@@ -2903,7 +3028,7 @@
         <v>20200740010</v>
       </c>
       <c r="B19" s="4" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C19">
         <v>67.58</v>
@@ -2914,7 +3039,7 @@
         <v>20200740011</v>
       </c>
       <c r="B20" s="4" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C20">
         <v>83.58</v>
@@ -2925,7 +3050,7 @@
         <v>20200740012</v>
       </c>
       <c r="B21" s="4" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C21">
         <v>78.78</v>
@@ -2936,7 +3061,7 @@
         <v>20200740013</v>
       </c>
       <c r="B22" s="4" t="s">
-        <v>45</v>
+        <v>64</v>
       </c>
       <c r="C22">
         <v>75.38</v>
@@ -2954,12 +3079,12 @@
   <dimension ref="A1:B9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A7" sqref="A7"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="16.5" outlineLevelCol="1"/>
+  <sheetFormatPr defaultColWidth="9.06666666666667" defaultRowHeight="15" outlineLevelCol="1"/>
   <cols>
-    <col min="1" max="1" width="9.06666666666667" style="1"/>
+    <col min="1" max="1" width="11.5" style="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2">
@@ -2967,72 +3092,137 @@
         <v>21</v>
       </c>
       <c r="B1" t="s">
-        <v>60</v>
+        <v>79</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" s="1" t="s">
+        <v>24</v>
+      </c>
+      <c r="B2" s="4" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B3" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B4" s="4" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2">
+      <c r="A5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B5" s="4" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2">
+      <c r="A6" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B6" s="4" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2">
+      <c r="A7" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B7" s="4" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2">
+      <c r="A8" s="1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B8" s="4" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2">
+      <c r="A9" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="B9" s="4" t="s">
+        <v>77</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H10" sqref="H10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9" defaultRowHeight="15" outlineLevelCol="1"/>
+  <sheetData>
+    <row r="1" spans="1:2">
+      <c r="A1" t="s">
+        <v>131</v>
+      </c>
+      <c r="B1" t="s">
+        <v>132</v>
       </c>
     </row>
     <row r="2" spans="1:2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="4" t="s">
-        <v>45</v>
+      <c r="B2">
+        <v>123456</v>
       </c>
     </row>
     <row r="3" spans="1:2">
       <c r="A3" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2">
-      <c r="A4" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B4" s="4" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2">
-      <c r="A5" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B5" s="4" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2">
-      <c r="A6" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B6" s="4" t="s">
-        <v>52</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2">
-      <c r="A7" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" s="4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2">
-      <c r="A8" s="1" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" s="4" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2">
-      <c r="A9" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" s="4" t="s">
-        <v>58</v>
-      </c>
+      <c r="B3">
+        <v>234567</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1">
+      <c r="A4" s="1"/>
+    </row>
+    <row r="5" spans="1:1">
+      <c r="A5" s="1"/>
+    </row>
+    <row r="6" spans="1:1">
+      <c r="A6" s="1"/>
+    </row>
+    <row r="7" spans="1:1">
+      <c r="A7" s="1"/>
+    </row>
+    <row r="8" spans="1:1">
+      <c r="A8" s="1"/>
+    </row>
+    <row r="9" spans="1:1">
+      <c r="A9" s="1"/>
+    </row>
+    <row r="10" spans="1:1">
+      <c r="A10" s="1"/>
+    </row>
+    <row r="11" spans="1:1">
+      <c r="A11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>

</xml_diff>